<commit_message>
switch to system user prompts
</commit_message>
<xml_diff>
--- a/docs/ContractAIForm.xlsx
+++ b/docs/ContractAIForm.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Projects\contractzlab\backend\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CFE373F2-4AFC-4C5D-8957-312BC9A0192D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4757C54-51D6-40D4-A021-D3F4AD4C4A74}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{CD81AD7E-50B5-FC4F-9C6A-67CD5946F7A6}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{CD81AD7E-50B5-FC4F-9C6A-67CD5946F7A6}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="86">
   <si>
     <t>Objet</t>
   </si>
@@ -354,19 +354,19 @@
     <t>sub_clause</t>
   </si>
   <si>
-    <t>prompt</t>
-  </si>
-  <si>
-    <t>Generate a Legal Document based on the draft pdf file and a desired output.
-Match the output format provided in clauses and subclaues
-Expand each clause and subclause into a comprehensive legal document format
-Language: Deduct from file.
-[pdf file]
-${pdfFile}
-[/pdf file]
-[output]
+    <t>system_prompt</t>
+  </si>
+  <si>
+    <t>user_prompt</t>
+  </si>
+  <si>
+    <t>${pdfFile}</t>
+  </si>
+  <si>
+    <t>Fill this csv spreedsheet with answers based on the provided legal document
+[csv]
 ${form}
-[/output]</t>
+[/csv]</t>
   </si>
 </sst>
 </file>
@@ -551,6 +551,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -568,12 +574,6 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -888,458 +888,478 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B27D1D9B-626C-5D44-B6AA-C9BCFC29F97C}">
-  <dimension ref="A1:K28"/>
+  <dimension ref="A1:L28"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="75" workbookViewId="0">
-      <selection activeCell="G19" sqref="G19"/>
+      <selection activeCell="G2" sqref="G2:G14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="7" max="7" width="71.625" customWidth="1"/>
-    <col min="8" max="8" width="23.625" customWidth="1"/>
-    <col min="9" max="9" width="45.375" customWidth="1"/>
-    <col min="10" max="10" width="113.625" style="8" customWidth="1"/>
-    <col min="11" max="11" width="96.375" customWidth="1"/>
+    <col min="7" max="7" width="39" customWidth="1"/>
+    <col min="8" max="8" width="71.625" customWidth="1"/>
+    <col min="9" max="9" width="23.625" customWidth="1"/>
+    <col min="10" max="10" width="45.375" customWidth="1"/>
+    <col min="11" max="11" width="113.625" style="8" customWidth="1"/>
+    <col min="12" max="12" width="96.375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="38.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" ht="38.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>77</v>
       </c>
       <c r="B1" t="s">
         <v>79</v>
       </c>
-      <c r="C1" s="16" t="s">
+      <c r="C1" s="9" t="s">
         <v>74</v>
       </c>
-      <c r="D1" s="16" t="s">
+      <c r="D1" s="9" t="s">
         <v>75</v>
       </c>
-      <c r="E1" s="16" t="s">
+      <c r="E1" s="9" t="s">
         <v>76</v>
       </c>
       <c r="F1" t="s">
         <v>66</v>
       </c>
-      <c r="G1" s="17" t="s">
+      <c r="G1" s="10" t="s">
         <v>82</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="H1" s="10" t="s">
+        <v>83</v>
+      </c>
+      <c r="I1" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="J1" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="J1" s="5" t="s">
+      <c r="K1" s="5" t="s">
         <v>68</v>
       </c>
-      <c r="K1" s="3" t="s">
+      <c r="L1" s="3" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="2" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="13" t="s">
+    <row r="2" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="15" t="s">
         <v>78</v>
       </c>
-      <c r="B2" s="13" t="s">
+      <c r="B2" s="15" t="s">
         <v>73</v>
       </c>
-      <c r="C2" s="13" t="s">
+      <c r="C2" s="15" t="s">
         <v>69</v>
       </c>
-      <c r="D2" s="13" t="s">
+      <c r="D2" s="15" t="s">
         <v>70</v>
       </c>
-      <c r="E2" s="13" t="s">
+      <c r="E2" s="15" t="s">
         <v>71</v>
       </c>
-      <c r="F2" s="13" t="s">
+      <c r="F2" s="15" t="s">
         <v>72</v>
       </c>
-      <c r="G2" s="13" t="s">
-        <v>83</v>
-      </c>
-      <c r="H2" s="10" t="s">
+      <c r="G2" s="15" t="s">
+        <v>85</v>
+      </c>
+      <c r="H2" s="15" t="s">
+        <v>84</v>
+      </c>
+      <c r="I2" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="I2" s="2"/>
-      <c r="J2" s="7" t="s">
+      <c r="J2" s="2"/>
+      <c r="K2" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="K2" s="3" t="s">
+      <c r="L2" s="3" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="14"/>
-      <c r="B3" s="14"/>
-      <c r="C3" s="14"/>
-      <c r="D3" s="14"/>
-      <c r="E3" s="14"/>
-      <c r="F3" s="14"/>
-      <c r="G3" s="14"/>
-      <c r="H3" s="11"/>
-      <c r="I3" s="2"/>
-      <c r="J3" s="5"/>
-      <c r="K3" s="3"/>
-    </row>
-    <row r="4" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="14"/>
-      <c r="B4" s="14"/>
-      <c r="C4" s="14"/>
-      <c r="D4" s="14"/>
-      <c r="E4" s="14"/>
-      <c r="F4" s="14"/>
-      <c r="G4" s="14"/>
-      <c r="H4" s="12"/>
-      <c r="I4" s="2"/>
-      <c r="J4" s="5"/>
-      <c r="K4" s="3"/>
-    </row>
-    <row r="5" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="14"/>
-      <c r="B5" s="14"/>
-      <c r="C5" s="14"/>
-      <c r="D5" s="14"/>
-      <c r="E5" s="14"/>
-      <c r="F5" s="14"/>
-      <c r="G5" s="14"/>
-      <c r="H5" s="1" t="s">
+    <row r="3" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="16"/>
+      <c r="B3" s="16"/>
+      <c r="C3" s="16"/>
+      <c r="D3" s="16"/>
+      <c r="E3" s="16"/>
+      <c r="F3" s="16"/>
+      <c r="G3" s="16"/>
+      <c r="H3" s="16"/>
+      <c r="I3" s="13"/>
+      <c r="J3" s="2"/>
+      <c r="K3" s="5"/>
+      <c r="L3" s="3"/>
+    </row>
+    <row r="4" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="16"/>
+      <c r="B4" s="16"/>
+      <c r="C4" s="16"/>
+      <c r="D4" s="16"/>
+      <c r="E4" s="16"/>
+      <c r="F4" s="16"/>
+      <c r="G4" s="16"/>
+      <c r="H4" s="16"/>
+      <c r="I4" s="14"/>
+      <c r="J4" s="2"/>
+      <c r="K4" s="5"/>
+      <c r="L4" s="3"/>
+    </row>
+    <row r="5" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="16"/>
+      <c r="B5" s="16"/>
+      <c r="C5" s="16"/>
+      <c r="D5" s="16"/>
+      <c r="E5" s="16"/>
+      <c r="F5" s="16"/>
+      <c r="G5" s="16"/>
+      <c r="H5" s="16"/>
+      <c r="I5" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="I5" s="4" t="s">
+      <c r="J5" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="J5" s="5" t="s">
+      <c r="K5" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="K5" s="3" t="s">
+      <c r="L5" s="3" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="14"/>
-      <c r="B6" s="14"/>
-      <c r="C6" s="14"/>
-      <c r="D6" s="14"/>
-      <c r="E6" s="14"/>
-      <c r="F6" s="14"/>
-      <c r="G6" s="14"/>
-      <c r="H6" s="9" t="s">
+    <row r="6" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="16"/>
+      <c r="B6" s="16"/>
+      <c r="C6" s="16"/>
+      <c r="D6" s="16"/>
+      <c r="E6" s="16"/>
+      <c r="F6" s="16"/>
+      <c r="G6" s="16"/>
+      <c r="H6" s="16"/>
+      <c r="I6" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="I6" s="2" t="s">
+      <c r="J6" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="J6" s="5" t="s">
+      <c r="K6" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="K6" s="3" t="s">
+      <c r="L6" s="3" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="14"/>
-      <c r="B7" s="14"/>
-      <c r="C7" s="14"/>
-      <c r="D7" s="14"/>
-      <c r="E7" s="14"/>
-      <c r="F7" s="14"/>
-      <c r="G7" s="14"/>
-      <c r="H7" s="9"/>
-      <c r="I7" s="2" t="s">
+    <row r="7" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="16"/>
+      <c r="B7" s="16"/>
+      <c r="C7" s="16"/>
+      <c r="D7" s="16"/>
+      <c r="E7" s="16"/>
+      <c r="F7" s="16"/>
+      <c r="G7" s="16"/>
+      <c r="H7" s="16"/>
+      <c r="I7" s="11"/>
+      <c r="J7" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="J7" s="7" t="s">
+      <c r="K7" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="K7" s="3" t="s">
+      <c r="L7" s="3" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="8" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="14"/>
-      <c r="B8" s="14"/>
-      <c r="C8" s="14"/>
-      <c r="D8" s="14"/>
-      <c r="E8" s="14"/>
-      <c r="F8" s="14"/>
-      <c r="G8" s="14"/>
-      <c r="H8" s="9"/>
-      <c r="I8" s="2" t="s">
+    <row r="8" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="16"/>
+      <c r="B8" s="16"/>
+      <c r="C8" s="16"/>
+      <c r="D8" s="16"/>
+      <c r="E8" s="16"/>
+      <c r="F8" s="16"/>
+      <c r="G8" s="16"/>
+      <c r="H8" s="16"/>
+      <c r="I8" s="11"/>
+      <c r="J8" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="J8" s="5" t="s">
+      <c r="K8" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="K8" s="3" t="s">
+      <c r="L8" s="3" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="9" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="14"/>
-      <c r="B9" s="14"/>
-      <c r="C9" s="14"/>
-      <c r="D9" s="14"/>
-      <c r="E9" s="14"/>
-      <c r="F9" s="14"/>
-      <c r="G9" s="14"/>
-      <c r="H9" s="10" t="s">
+    <row r="9" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="16"/>
+      <c r="B9" s="16"/>
+      <c r="C9" s="16"/>
+      <c r="D9" s="16"/>
+      <c r="E9" s="16"/>
+      <c r="F9" s="16"/>
+      <c r="G9" s="16"/>
+      <c r="H9" s="16"/>
+      <c r="I9" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="I9" s="2" t="s">
+      <c r="J9" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="J9" s="5" t="s">
+      <c r="K9" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="K9" s="3" t="s">
+      <c r="L9" s="3" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="10" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="14"/>
-      <c r="B10" s="14"/>
-      <c r="C10" s="14"/>
-      <c r="D10" s="14"/>
-      <c r="E10" s="14"/>
-      <c r="F10" s="14"/>
-      <c r="G10" s="14"/>
-      <c r="H10" s="11"/>
-      <c r="I10" s="2" t="s">
+    <row r="10" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="16"/>
+      <c r="B10" s="16"/>
+      <c r="C10" s="16"/>
+      <c r="D10" s="16"/>
+      <c r="E10" s="16"/>
+      <c r="F10" s="16"/>
+      <c r="G10" s="16"/>
+      <c r="H10" s="16"/>
+      <c r="I10" s="13"/>
+      <c r="J10" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="J10" s="5" t="s">
+      <c r="K10" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="K10" s="3" t="s">
+      <c r="L10" s="3" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="11" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="14"/>
-      <c r="B11" s="14"/>
-      <c r="C11" s="14"/>
-      <c r="D11" s="14"/>
-      <c r="E11" s="14"/>
-      <c r="F11" s="14"/>
-      <c r="G11" s="14"/>
-      <c r="H11" s="11"/>
-      <c r="I11" s="2" t="s">
+    <row r="11" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="16"/>
+      <c r="B11" s="16"/>
+      <c r="C11" s="16"/>
+      <c r="D11" s="16"/>
+      <c r="E11" s="16"/>
+      <c r="F11" s="16"/>
+      <c r="G11" s="16"/>
+      <c r="H11" s="16"/>
+      <c r="I11" s="13"/>
+      <c r="J11" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="J11" s="5" t="s">
+      <c r="K11" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="K11" s="3" t="s">
+      <c r="L11" s="3" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="12" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="14"/>
-      <c r="B12" s="14"/>
-      <c r="C12" s="14"/>
-      <c r="D12" s="14"/>
-      <c r="E12" s="14"/>
-      <c r="F12" s="14"/>
-      <c r="G12" s="14"/>
-      <c r="H12" s="11"/>
-      <c r="I12" s="2" t="s">
+    <row r="12" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="16"/>
+      <c r="B12" s="16"/>
+      <c r="C12" s="16"/>
+      <c r="D12" s="16"/>
+      <c r="E12" s="16"/>
+      <c r="F12" s="16"/>
+      <c r="G12" s="16"/>
+      <c r="H12" s="16"/>
+      <c r="I12" s="13"/>
+      <c r="J12" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="J12" s="5" t="s">
+      <c r="K12" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="K12" s="3" t="s">
+      <c r="L12" s="3" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="13" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="14"/>
-      <c r="B13" s="14"/>
-      <c r="C13" s="14"/>
-      <c r="D13" s="14"/>
-      <c r="E13" s="14"/>
-      <c r="F13" s="14"/>
-      <c r="G13" s="14"/>
-      <c r="H13" s="12"/>
-      <c r="I13" s="6" t="s">
+    <row r="13" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="16"/>
+      <c r="B13" s="16"/>
+      <c r="C13" s="16"/>
+      <c r="D13" s="16"/>
+      <c r="E13" s="16"/>
+      <c r="F13" s="16"/>
+      <c r="G13" s="16"/>
+      <c r="H13" s="16"/>
+      <c r="I13" s="14"/>
+      <c r="J13" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="J13" s="5" t="s">
+      <c r="K13" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="K13" s="3" t="s">
+      <c r="L13" s="3" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="14" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="15"/>
-      <c r="B14" s="15"/>
-      <c r="C14" s="15"/>
-      <c r="D14" s="15"/>
-      <c r="E14" s="15"/>
-      <c r="F14" s="15"/>
-      <c r="G14" s="15"/>
-      <c r="H14" s="9" t="s">
+    <row r="14" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="17"/>
+      <c r="B14" s="17"/>
+      <c r="C14" s="17"/>
+      <c r="D14" s="17"/>
+      <c r="E14" s="17"/>
+      <c r="F14" s="17"/>
+      <c r="G14" s="17"/>
+      <c r="H14" s="17"/>
+      <c r="I14" s="11" t="s">
         <v>32</v>
       </c>
-      <c r="I14" s="2" t="s">
+      <c r="J14" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="J14" s="5" t="s">
+      <c r="K14" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="K14" s="3" t="s">
+      <c r="L14" s="3" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="15" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="H15" s="9"/>
-      <c r="I15" s="2" t="s">
+    <row r="15" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I15" s="11"/>
+      <c r="J15" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="J15" s="5" t="s">
+      <c r="K15" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="K15" s="3" t="s">
+      <c r="L15" s="3" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="16" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="H16" s="9" t="s">
+    <row r="16" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I16" s="11" t="s">
         <v>39</v>
       </c>
-      <c r="I16" s="2" t="s">
+      <c r="J16" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="J16" s="5" t="s">
+      <c r="K16" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="K16" s="3"/>
-    </row>
-    <row r="17" spans="8:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="H17" s="9"/>
-      <c r="I17" s="2" t="s">
+      <c r="L16" s="3"/>
+    </row>
+    <row r="17" spans="9:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I17" s="11"/>
+      <c r="J17" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="J17" s="5" t="s">
+      <c r="K17" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="K17" s="3"/>
-    </row>
-    <row r="18" spans="8:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="H18" s="9"/>
-      <c r="I18" s="2" t="s">
+      <c r="L17" s="3"/>
+    </row>
+    <row r="18" spans="9:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I18" s="11"/>
+      <c r="J18" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="J18" s="5" t="s">
+      <c r="K18" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="K18" s="3" t="s">
+      <c r="L18" s="3" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="19" spans="8:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="H19" s="9"/>
-      <c r="I19" s="2" t="s">
+    <row r="19" spans="9:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I19" s="11"/>
+      <c r="J19" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="J19" s="5" t="s">
+      <c r="K19" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="K19" s="3" t="s">
+      <c r="L19" s="3" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="20" spans="8:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="H20" s="9" t="s">
+    <row r="20" spans="9:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I20" s="11" t="s">
         <v>50</v>
       </c>
-      <c r="I20" s="2" t="s">
+      <c r="J20" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="J20" s="5" t="s">
+      <c r="K20" s="5" t="s">
         <v>52</v>
       </c>
-      <c r="K20" s="3" t="s">
+      <c r="L20" s="3" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="21" spans="8:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="H21" s="9"/>
-      <c r="I21" s="2" t="s">
+    <row r="21" spans="9:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I21" s="11"/>
+      <c r="J21" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="J21" s="5" t="s">
+      <c r="K21" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="K21" s="3"/>
-    </row>
-    <row r="22" spans="8:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="H22" s="1" t="s">
+      <c r="L21" s="3"/>
+    </row>
+    <row r="22" spans="9:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I22" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="I22" s="2"/>
-      <c r="J22" s="5" t="s">
+      <c r="J22" s="2"/>
+      <c r="K22" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="K22" s="3"/>
-    </row>
-    <row r="23" spans="8:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="H23" s="9" t="s">
+      <c r="L22" s="3"/>
+    </row>
+    <row r="23" spans="9:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I23" s="11" t="s">
         <v>58</v>
       </c>
-      <c r="I23" s="2" t="s">
+      <c r="J23" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="J23" s="5" t="s">
+      <c r="K23" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="K23" s="3"/>
-    </row>
-    <row r="24" spans="8:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="H24" s="9"/>
-      <c r="I24" s="2" t="s">
+      <c r="L23" s="3"/>
+    </row>
+    <row r="24" spans="9:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I24" s="11"/>
+      <c r="J24" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="J24" s="5" t="s">
+      <c r="K24" s="5" t="s">
         <v>62</v>
       </c>
-      <c r="K24" s="3" t="s">
+      <c r="L24" s="3" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="25" spans="8:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="H25" s="9"/>
-      <c r="I25" s="2"/>
-      <c r="J25" s="5" t="s">
+    <row r="25" spans="9:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I25" s="11"/>
+      <c r="J25" s="2"/>
+      <c r="K25" s="5" t="s">
         <v>64</v>
       </c>
-      <c r="K25" s="3" t="s">
+      <c r="L25" s="3" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="26" spans="8:11" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="27" spans="8:11" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="28" spans="8:11" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="26" spans="9:12" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="27" spans="9:12" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="28" spans="9:12" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
-  <mergeCells count="14">
+  <mergeCells count="15">
     <mergeCell ref="A2:A14"/>
-    <mergeCell ref="G2:G14"/>
+    <mergeCell ref="H2:H14"/>
     <mergeCell ref="E2:E14"/>
     <mergeCell ref="D2:D14"/>
     <mergeCell ref="F2:F14"/>
     <mergeCell ref="C2:C14"/>
     <mergeCell ref="B2:B14"/>
-    <mergeCell ref="H23:H25"/>
-    <mergeCell ref="H20:H21"/>
-    <mergeCell ref="H2:H4"/>
-    <mergeCell ref="H6:H8"/>
-    <mergeCell ref="H9:H13"/>
-    <mergeCell ref="H14:H15"/>
-    <mergeCell ref="H16:H19"/>
+    <mergeCell ref="G2:G14"/>
+    <mergeCell ref="I23:I25"/>
+    <mergeCell ref="I20:I21"/>
+    <mergeCell ref="I2:I4"/>
+    <mergeCell ref="I6:I8"/>
+    <mergeCell ref="I9:I13"/>
+    <mergeCell ref="I14:I15"/>
+    <mergeCell ref="I16:I19"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>